<commit_message>
5-commit by lesson13 edit message text
</commit_message>
<xml_diff>
--- a/Lesson13_TelegramBots/src/main/resources/documents/customers.xlsx
+++ b/Lesson13_TelegramBots/src/main/resources/documents/customers.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
   <si>
     <t>Chat id</t>
   </si>
@@ -216,6 +216,18 @@
   </si>
   <si>
     <t>+998909152526</t>
+  </si>
+  <si>
+    <t>616525392</t>
+  </si>
+  <si>
+    <t>Nurbek</t>
+  </si>
+  <si>
+    <t>Boboyev</t>
+  </si>
+  <si>
+    <t>+998946696195</t>
   </si>
 </sst>
 </file>
@@ -260,7 +272,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -536,6 +548,20 @@
         <v>67</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>